<commit_message>
Update documentation dqc_0104 and list of axes spreadsheet
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0104/DQC_0104_ListOfAxes.xlsx
+++ b/docs/DQC_US_0104/DQC_0104_ListOfAxes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aicpa-my.sharepoint.com/personal/abeers_aicpa_org/Documents/XBRL/Data Quality Consortium/Committee Meetings/2020/October 2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DJT\Documents\GitHub\DQC\dqc_us_rules\docs\DQC_US_0104\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BD95262-699C-48CF-B5E0-AC48C7251E7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930BB55A-8C1B-4B47-8908-B8ADAEA40F76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45285" yWindow="5820" windowWidth="17160" windowHeight="10965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,26 @@
     <t>Segment consolidation items [axis]</t>
   </si>
   <si>
+    <t>DQC_0104.9555</t>
+  </si>
+  <si>
+    <t>SegmentsAxis</t>
+  </si>
+  <si>
+    <t>Segments [axis]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Descendants of EliminationOfIntersegmentAmountsMember and UnallocatedAmountsMember and MaterialReconcilingItemsMember in definition linkbase.
+CorporateReconcilingItemsAndEliminationsMember, 
+CorporateAndReconcilingItemsMember, 
+CorporateAndEliminationsMember, 
+EliminationsAndReconcilingItemsMember, 
+OperatingSegmentsAndCorporateNonSegmentMember, 
+OperatingSegmentsAndUnallocatedMember
+OperatingSegmentsExcludingIntersegmentEliminationMember,
+CorporateNonSegmentMember,
+GeographyEliminationsMember,
+OtherNonSegmentMember
 CorporateReconcilingItemsAndEliminationsMember, 
 CorporateAndReconcilingItemsMember, 
 CorporateAndEliminationsMember, 
@@ -126,15 +145,6 @@
 GeographyEliminationsMember,
 OtherNonSegmentMember
 </t>
-  </si>
-  <si>
-    <t>DQC_0104.9555</t>
-  </si>
-  <si>
-    <t>SegmentsAxis</t>
-  </si>
-  <si>
-    <t>Segments [axis]</t>
   </si>
 </sst>
 </file>
@@ -570,24 +580,24 @@
   </sheetPr>
   <dimension ref="A1:AD12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="H2" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="54" customWidth="1"/>
     <col min="5" max="5" width="47" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" customWidth="1"/>
-    <col min="7" max="7" width="46.88671875" customWidth="1"/>
-    <col min="8" max="8" width="31.44140625" customWidth="1"/>
-    <col min="10" max="10" width="54.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="46.85546875" customWidth="1"/>
+    <col min="8" max="8" width="31.42578125" customWidth="1"/>
+    <col min="10" max="10" width="54.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -642,7 +652,7 @@
       <c r="AB1" s="3"/>
       <c r="AC1" s="3"/>
     </row>
-    <row r="2" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -673,7 +683,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
@@ -704,7 +714,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
@@ -733,7 +743,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="276" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
@@ -757,16 +767,16 @@
       <c r="I5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="6" t="s">
-        <v>31</v>
+      <c r="J5" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="K5" s="6">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>13</v>
@@ -775,10 +785,10 @@
         <v>14</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>17</v>
@@ -793,7 +803,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -807,7 +817,7 @@
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
     </row>
-    <row r="8" spans="1:30" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
@@ -839,7 +849,7 @@
       <c r="AC8" s="11"/>
       <c r="AD8" s="11"/>
     </row>
-    <row r="11" spans="1:30" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -847,7 +857,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:30" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -862,6 +872,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100669C1DF1C9155E4C87633C75EE97BEC4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f5437fdcf964fc7da6521cca7e726ac1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fb8819a2-58ee-41ee-b9b3-dd3c6a0952ee" xmlns:ns4="e23a85b1-e437-4f93-afa6-4fdbf67bab64" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c573a22cf0fc1d1ac2770d4c9f50a8cb" ns3:_="" ns4:_="">
     <xsd:import namespace="fb8819a2-58ee-41ee-b9b3-dd3c6a0952ee"/>
@@ -1084,22 +1109,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DE76882-7E5B-44E0-B938-115949D68270}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{522857C3-D744-4824-8744-5F9507F9793B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F845976-458E-4441-A40C-349EBCFEC2DB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1116,21 +1143,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{522857C3-D744-4824-8744-5F9507F9793B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DE76882-7E5B-44E0-B938-115949D68270}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update documentation as approved & copyright
includes edits to xlsx files dqc_0104 and dqc_0015
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0104/DQC_0104_ListOfAxes.xlsx
+++ b/docs/DQC_US_0104/DQC_0104_ListOfAxes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DJT\Documents\GitHub\DQC\dqc_us_rules\docs\DQC_US_0104\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DJT\Documents\GitHub\davidtauriello\dqc_us_rules\docs\DQC_US_0104\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930BB55A-8C1B-4B47-8908-B8ADAEA40F76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D93CE2D-5D3E-4BCE-89F6-A50A48B834A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45285" yWindow="5820" windowWidth="17160" windowHeight="10965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44430" yWindow="4290" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,9 +79,6 @@
     <t>Limited</t>
   </si>
   <si>
-    <t>Descendants of NoncurrentAssetsHeldForSaleMember and DisposalGroupsClassifiedAsHeldForSaleMember in definition linkbase</t>
-  </si>
-  <si>
     <t>DQC_0104.9552</t>
   </si>
   <si>
@@ -124,22 +121,17 @@
     <t>Segments [axis]</t>
   </si>
   <si>
+    <t>Descendants of NoncurrentAssetsHeldForSaleMember, AssetsAndLiabilitiesClassifiedAsHeldForSaleMember and DisposalGroupsClassifiedAsHeldForSaleMember in definition linkbase.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Descendants of EliminationOfIntersegmentAmountsMember and UnallocatedAmountsMember and MaterialReconcilingItemsMember in definition linkbase.
+Descendants of OperatingSegmentsMember in the definition linkbase that are either called ReportableSubsegmentsMember or IntersubsegmentEliminationsMember.
 CorporateReconcilingItemsAndEliminationsMember, 
 CorporateAndReconcilingItemsMember, 
 CorporateAndEliminationsMember, 
 EliminationsAndReconcilingItemsMember, 
 OperatingSegmentsAndCorporateNonSegmentMember, 
 OperatingSegmentsAndUnallocatedMember
-OperatingSegmentsExcludingIntersegmentEliminationMember,
-CorporateNonSegmentMember,
-GeographyEliminationsMember,
-OtherNonSegmentMember
-CorporateReconcilingItemsAndEliminationsMember, 
-CorporateAndReconcilingItemsMember, 
-CorporateAndEliminationsMember, 
-EliminationsAndReconcilingItemsMember, 
-OperatingSegmentsAndCorporateNonSegmentMember, 
 OperatingSegmentsExcludingIntersegmentEliminationMember,
 CorporateNonSegmentMember,
 GeographyEliminationsMember,
@@ -580,9 +572,7 @@
   </sheetPr>
   <dimension ref="A1:AD12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H2" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -677,7 +667,7 @@
         <v>18</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="K2" s="4">
         <v>14</v>
@@ -685,7 +675,7 @@
     </row>
     <row r="3" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>13</v>
@@ -694,10 +684,10 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>17</v>
@@ -708,7 +698,7 @@
         <v>18</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3" s="6">
         <v>14</v>
@@ -716,7 +706,7 @@
     </row>
     <row r="4" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>13</v>
@@ -725,10 +715,10 @@
         <v>14</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>17</v>
@@ -736,16 +726,16 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="276" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" ht="204" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>13</v>
@@ -754,10 +744,10 @@
         <v>14</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>30</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>17</v>
@@ -776,7 +766,7 @@
     </row>
     <row r="6" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>13</v>
@@ -785,10 +775,10 @@
         <v>14</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>17</v>
@@ -872,21 +862,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100669C1DF1C9155E4C87633C75EE97BEC4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f5437fdcf964fc7da6521cca7e726ac1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fb8819a2-58ee-41ee-b9b3-dd3c6a0952ee" xmlns:ns4="e23a85b1-e437-4f93-afa6-4fdbf67bab64" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c573a22cf0fc1d1ac2770d4c9f50a8cb" ns3:_="" ns4:_="">
     <xsd:import namespace="fb8819a2-58ee-41ee-b9b3-dd3c6a0952ee"/>
@@ -1109,24 +1084,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DE76882-7E5B-44E0-B938-115949D68270}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{522857C3-D744-4824-8744-5F9507F9793B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F845976-458E-4441-A40C-349EBCFEC2DB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1143,4 +1116,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{522857C3-D744-4824-8744-5F9507F9793B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DE76882-7E5B-44E0-B938-115949D68270}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Merge for v14.0.0 DQC Approved (#519)
* Updated rules for DQC 15 None issue.

* Updated 0004 and 0102 for comparison of values

Only do comparison with nonils values.

* Update resources.zip

* Recompiled version 14

* Updated rule 84 to make message easier to read in excel.

* Added 2021 rules

Added 2021 rules to the DQC ruleset

* Create dqc-us-2021-V14-ruleset.zip

Added ruleset for 2021 taxonomy

* Updated rule 104 to allow extensions on operating items.

* Update ifrs_effective_dates.csv

* Update effective_dates.csv

* Update resources.zip

* Update version.xule

* Updated ruleset files for V14

* Update documentation as approved & copyright

includes edits to xlsx files dqc_0104 and dqc_0015

Co-authored-by: campbellpryde
</commit_message>
<xml_diff>
--- a/docs/DQC_US_0104/DQC_0104_ListOfAxes.xlsx
+++ b/docs/DQC_US_0104/DQC_0104_ListOfAxes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DJT\Documents\GitHub\DQC\dqc_us_rules\docs\DQC_US_0104\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DJT\Documents\GitHub\davidtauriello\dqc_us_rules\docs\DQC_US_0104\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930BB55A-8C1B-4B47-8908-B8ADAEA40F76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D93CE2D-5D3E-4BCE-89F6-A50A48B834A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45285" yWindow="5820" windowWidth="17160" windowHeight="10965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44430" yWindow="4290" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,9 +79,6 @@
     <t>Limited</t>
   </si>
   <si>
-    <t>Descendants of NoncurrentAssetsHeldForSaleMember and DisposalGroupsClassifiedAsHeldForSaleMember in definition linkbase</t>
-  </si>
-  <si>
     <t>DQC_0104.9552</t>
   </si>
   <si>
@@ -124,22 +121,17 @@
     <t>Segments [axis]</t>
   </si>
   <si>
+    <t>Descendants of NoncurrentAssetsHeldForSaleMember, AssetsAndLiabilitiesClassifiedAsHeldForSaleMember and DisposalGroupsClassifiedAsHeldForSaleMember in definition linkbase.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Descendants of EliminationOfIntersegmentAmountsMember and UnallocatedAmountsMember and MaterialReconcilingItemsMember in definition linkbase.
+Descendants of OperatingSegmentsMember in the definition linkbase that are either called ReportableSubsegmentsMember or IntersubsegmentEliminationsMember.
 CorporateReconcilingItemsAndEliminationsMember, 
 CorporateAndReconcilingItemsMember, 
 CorporateAndEliminationsMember, 
 EliminationsAndReconcilingItemsMember, 
 OperatingSegmentsAndCorporateNonSegmentMember, 
 OperatingSegmentsAndUnallocatedMember
-OperatingSegmentsExcludingIntersegmentEliminationMember,
-CorporateNonSegmentMember,
-GeographyEliminationsMember,
-OtherNonSegmentMember
-CorporateReconcilingItemsAndEliminationsMember, 
-CorporateAndReconcilingItemsMember, 
-CorporateAndEliminationsMember, 
-EliminationsAndReconcilingItemsMember, 
-OperatingSegmentsAndCorporateNonSegmentMember, 
 OperatingSegmentsExcludingIntersegmentEliminationMember,
 CorporateNonSegmentMember,
 GeographyEliminationsMember,
@@ -580,9 +572,7 @@
   </sheetPr>
   <dimension ref="A1:AD12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H2" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -677,7 +667,7 @@
         <v>18</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="K2" s="4">
         <v>14</v>
@@ -685,7 +675,7 @@
     </row>
     <row r="3" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>13</v>
@@ -694,10 +684,10 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>17</v>
@@ -708,7 +698,7 @@
         <v>18</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3" s="6">
         <v>14</v>
@@ -716,7 +706,7 @@
     </row>
     <row r="4" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>13</v>
@@ -725,10 +715,10 @@
         <v>14</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>17</v>
@@ -736,16 +726,16 @@
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="276" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" ht="204" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>13</v>
@@ -754,10 +744,10 @@
         <v>14</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>30</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>17</v>
@@ -776,7 +766,7 @@
     </row>
     <row r="6" spans="1:30" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>13</v>
@@ -785,10 +775,10 @@
         <v>14</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>33</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>17</v>
@@ -872,21 +862,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100669C1DF1C9155E4C87633C75EE97BEC4" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f5437fdcf964fc7da6521cca7e726ac1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fb8819a2-58ee-41ee-b9b3-dd3c6a0952ee" xmlns:ns4="e23a85b1-e437-4f93-afa6-4fdbf67bab64" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c573a22cf0fc1d1ac2770d4c9f50a8cb" ns3:_="" ns4:_="">
     <xsd:import namespace="fb8819a2-58ee-41ee-b9b3-dd3c6a0952ee"/>
@@ -1109,24 +1084,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DE76882-7E5B-44E0-B938-115949D68270}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{522857C3-D744-4824-8744-5F9507F9793B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F845976-458E-4441-A40C-349EBCFEC2DB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1143,4 +1116,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{522857C3-D744-4824-8744-5F9507F9793B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DE76882-7E5B-44E0-B938-115949D68270}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>